<commit_message>
LTSpice triangular wave simulation working with appropiate values!
</commit_message>
<xml_diff>
--- a/Ej8/Others/eleccion-componentes.xlsx
+++ b/Ej8/Others/eleccion-componentes.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Clock3" sheetId="1" r:id="rId1"/>
     <sheet name="Clock2" sheetId="2" r:id="rId2"/>
     <sheet name="Clock1" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
+    <sheet name="Clock2final" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
   <si>
     <t>CLOCK 1</t>
   </si>
@@ -195,6 +195,21 @@
   <si>
     <t>t_low(f_max)</t>
   </si>
+  <si>
+    <t>Medicion</t>
+  </si>
+  <si>
+    <t>β</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>f (Hz)</t>
+  </si>
+  <si>
+    <t>preset</t>
+  </si>
 </sst>
 </file>
 
@@ -204,13 +219,19 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="##0.00E+00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -513,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -580,15 +601,16 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z604"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -909,14 +931,14 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="F2" s="57" t="s">
+      <c r="B2" s="57"/>
+      <c r="F2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="57"/>
+      <c r="G2" s="58"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -980,10 +1002,10 @@
       <c r="G5" s="3">
         <v>4.6999999999999999E-6</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="L5" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="56"/>
+      <c r="M5" s="57"/>
       <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -1027,16 +1049,16 @@
         <v>52</v>
       </c>
       <c r="V6" s="1"/>
-      <c r="W6" s="58" t="s">
+      <c r="W6" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="X6" s="58" t="s">
+      <c r="X6" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="Y6" s="58" t="s">
+      <c r="Y6" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="Z6" s="58" t="s">
+      <c r="Z6" s="56" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10616,7 +10638,7 @@
   <dimension ref="A5:R36"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11306,7 +11328,7 @@
   <dimension ref="A1:M291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15925,25 +15947,84 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4.7E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B3/(B3+B2)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="54">
+        <f>1/(B1*2*B4*LN((1+B5)/(1-B5)))</f>
+        <v>19366.792055890157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>